<commit_message>
Email using .env EMAIL_USER & EMAIL_PASS
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -524,9 +524,29 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Swapnil Durafe</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Paneer</v>
+      </c>
+      <c r="C8" t="str">
+        <v>16/7/2025, 12:19:45 am</v>
+      </c>
+      <c r="D8" t="str">
+        <v>D/4, C-204, Laxmi Park-1, Lokmanya Nagar, Thane-west</v>
+      </c>
+      <c r="E8" t="str">
+        <v>09372979927</v>
+      </c>
+      <c r="F8" t="str">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>